<commit_message>
Fix tests ExcelReaderStrategy, ParseCommon and FileParserFactory
</commit_message>
<xml_diff>
--- a/dataset-service/testExcelFile.xlsx
+++ b/dataset-service/testExcelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>BWID</t>
   </si>
@@ -26,6 +26,12 @@
     <t>EndDateS</t>
   </si>
   <si>
+    <t>DummiColumn</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>ES511M270688</t>
   </si>
   <si>
@@ -36,6 +42,12 @@
   </si>
   <si>
     <t>19/07/2018</t>
+  </si>
+  <si>
+    <t>DummiCell</t>
+  </si>
+  <si>
+    <t>ThisValueShouldNotBeReaden</t>
   </si>
   <si>
     <t>ES512M118746</t>
@@ -92,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -111,44 +123,79 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>